<commit_message>
Made changes to include the following: 1. Add code and customer to beginning of all original files 2. If Credit Memo, add 3 new sheets: 1. CM Invoices that only includes invoices in which there is a Credit Memo. 2. Sales Receipts. 3. Journal Entries. 3. Add new reference numbers for Checks (ABB TR 00001) and Journal Entries (PMT 00001).
</commit_message>
<xml_diff>
--- a/ModelFiles/VRBO_04_2023-04_2023.xlsx
+++ b/ModelFiles/VRBO_04_2023-04_2023.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SupAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{248EF804-DC83-4F27-B85C-75A1B8D308E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{248EF804-DC83-4F27-B85C-75A1B8D308E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F843A2BD-E9B2-4D21-B81D-C835624B6035}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2445" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-2445" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PayoutSummaryReport_2023-04-01_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PayoutSummaryReport_2023-04-01_'!$A$1:$Q$78</definedName>
+  </definedNames>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -883,8 +899,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1718,14 +1734,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N68"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
+  <cols>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1778,7 +1805,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" hidden="1">
       <c r="A2">
         <v>2646992</v>
       </c>
@@ -1831,7 +1858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2647796</v>
       </c>
@@ -1884,7 +1911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" hidden="1">
       <c r="A4">
         <v>2653772</v>
       </c>
@@ -1937,7 +1964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>2660924</v>
       </c>
@@ -1990,7 +2017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>2661227</v>
       </c>
@@ -2043,7 +2070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>2661306</v>
       </c>
@@ -2096,7 +2123,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>2661622</v>
       </c>
@@ -2149,7 +2176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>2661622</v>
       </c>
@@ -2202,7 +2229,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>2661682</v>
       </c>
@@ -2255,7 +2282,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>2662813</v>
       </c>
@@ -2308,7 +2335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" hidden="1">
       <c r="A12">
         <v>2662844</v>
       </c>
@@ -2361,7 +2388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1">
       <c r="A13">
         <v>2662844</v>
       </c>
@@ -2414,7 +2441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" hidden="1">
       <c r="A14">
         <v>2663313</v>
       </c>
@@ -2467,7 +2494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>2663949</v>
       </c>
@@ -2520,7 +2547,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>2680053</v>
       </c>
@@ -2573,7 +2600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>2680053</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>2680053</v>
       </c>
@@ -2679,7 +2706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>2680053</v>
       </c>
@@ -2732,7 +2759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>2680053</v>
       </c>
@@ -2785,7 +2812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>2680053</v>
       </c>
@@ -2838,7 +2865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" hidden="1">
       <c r="A22">
         <v>2684531</v>
       </c>
@@ -2891,7 +2918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" hidden="1">
       <c r="A23">
         <v>2684559</v>
       </c>
@@ -2944,7 +2971,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" hidden="1">
       <c r="A24">
         <v>2721563</v>
       </c>
@@ -2997,7 +3024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" hidden="1">
       <c r="A25">
         <v>2721563</v>
       </c>
@@ -3050,7 +3077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" hidden="1">
       <c r="A26">
         <v>2721563</v>
       </c>
@@ -3103,7 +3130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" hidden="1">
       <c r="A27">
         <v>2769263</v>
       </c>
@@ -3156,7 +3183,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" hidden="1">
       <c r="A28">
         <v>2769263</v>
       </c>
@@ -3209,7 +3236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>2772370</v>
       </c>
@@ -3262,7 +3289,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" hidden="1">
       <c r="A30">
         <v>2797954</v>
       </c>
@@ -3315,7 +3342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" hidden="1">
       <c r="A31">
         <v>2868353</v>
       </c>
@@ -3368,7 +3395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>2879071</v>
       </c>
@@ -3421,7 +3448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>2879071</v>
       </c>
@@ -3474,7 +3501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" hidden="1">
       <c r="A34">
         <v>2916363</v>
       </c>
@@ -3527,7 +3554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" hidden="1">
       <c r="A35">
         <v>2916363</v>
       </c>
@@ -3580,7 +3607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" hidden="1">
       <c r="A36">
         <v>2916363</v>
       </c>
@@ -3633,7 +3660,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" hidden="1">
       <c r="A37">
         <v>3020005</v>
       </c>
@@ -3686,7 +3713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" hidden="1">
       <c r="A38">
         <v>3020005</v>
       </c>
@@ -3739,7 +3766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" hidden="1">
       <c r="A39">
         <v>3021015</v>
       </c>
@@ -3792,7 +3819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" hidden="1">
       <c r="A40">
         <v>3021082</v>
       </c>
@@ -3845,7 +3872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" hidden="1">
       <c r="A41">
         <v>3024064</v>
       </c>
@@ -3898,7 +3925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" hidden="1">
       <c r="A42">
         <v>3024064</v>
       </c>
@@ -3951,7 +3978,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" hidden="1">
       <c r="A43">
         <v>3024064</v>
       </c>
@@ -4004,7 +4031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" hidden="1">
       <c r="A44">
         <v>3024064</v>
       </c>
@@ -4057,7 +4084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" hidden="1">
       <c r="A45">
         <v>3025151</v>
       </c>
@@ -4110,7 +4137,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1">
       <c r="A46">
         <v>3030324</v>
       </c>
@@ -4163,7 +4190,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>3031250</v>
       </c>
@@ -4216,7 +4243,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" hidden="1">
       <c r="A48">
         <v>3031302</v>
       </c>
@@ -4269,7 +4296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>3036149</v>
       </c>
@@ -4322,7 +4349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>3036149</v>
       </c>
@@ -4375,7 +4402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>3036149</v>
       </c>
@@ -4428,7 +4455,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" hidden="1">
       <c r="A52">
         <v>3058087</v>
       </c>
@@ -4481,7 +4508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" hidden="1">
       <c r="A53">
         <v>3058087</v>
       </c>
@@ -4534,7 +4561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" hidden="1">
       <c r="A54">
         <v>3058087</v>
       </c>
@@ -4587,7 +4614,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" hidden="1">
       <c r="A55">
         <v>3058087</v>
       </c>
@@ -4640,7 +4667,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" hidden="1">
       <c r="A56">
         <v>3080225</v>
       </c>
@@ -4693,7 +4720,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17">
       <c r="A57">
         <v>3097466</v>
       </c>
@@ -4746,7 +4773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17">
       <c r="A58">
         <v>3116088</v>
       </c>
@@ -4799,7 +4826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" hidden="1">
       <c r="A59">
         <v>3117112</v>
       </c>
@@ -4852,7 +4879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" hidden="1">
       <c r="A60">
         <v>3117112</v>
       </c>
@@ -4905,7 +4932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" hidden="1">
       <c r="A61">
         <v>3138747</v>
       </c>
@@ -4958,7 +4985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" hidden="1">
       <c r="A62">
         <v>3138747</v>
       </c>
@@ -5011,7 +5038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" hidden="1">
       <c r="A63">
         <v>3138747</v>
       </c>
@@ -5064,7 +5091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17">
       <c r="A64">
         <v>3187869</v>
       </c>
@@ -5117,7 +5144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" hidden="1">
       <c r="A65">
         <v>3187979</v>
       </c>
@@ -5170,7 +5197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" hidden="1">
       <c r="A66">
         <v>3187979</v>
       </c>
@@ -5223,7 +5250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" hidden="1">
       <c r="A67">
         <v>3293721</v>
       </c>
@@ -5276,7 +5303,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17">
       <c r="A68">
         <v>3294127</v>
       </c>
@@ -5329,7 +5356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" hidden="1">
       <c r="A69">
         <v>4918827</v>
       </c>
@@ -5382,7 +5409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" hidden="1">
       <c r="A70">
         <v>4918827</v>
       </c>
@@ -5435,7 +5462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" hidden="1">
       <c r="A71">
         <v>4918827</v>
       </c>
@@ -5488,7 +5515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" hidden="1">
       <c r="A72">
         <v>4918827</v>
       </c>
@@ -5541,7 +5568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" hidden="1">
       <c r="A73">
         <v>4918827</v>
       </c>
@@ -5594,7 +5621,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" hidden="1">
       <c r="A74">
         <v>7435967</v>
       </c>
@@ -5647,7 +5674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" hidden="1">
       <c r="A75">
         <v>7435967</v>
       </c>
@@ -5700,7 +5727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" hidden="1">
       <c r="A76">
         <v>7468494</v>
       </c>
@@ -5753,7 +5780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" hidden="1">
       <c r="A77">
         <v>7481558</v>
       </c>
@@ -5806,7 +5833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" hidden="1">
       <c r="A78">
         <v>7502407</v>
       </c>
@@ -5860,11 +5887,54 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q78" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1117 Dogwood Dr N"/>
+        <filter val="1117 Dogwood Dr N B"/>
+        <filter val="1900 Cassandra Ln"/>
+        <filter val="3404 Burris St"/>
+        <filter val="4525 S Ocean Blvd"/>
+        <filter val="4655 Wild Iris Dr"/>
+        <filter val="4669 Wild Iris Dr 202"/>
+        <filter val="4709 Wild Iris Dr 204"/>
+        <filter val="4726 Cloisters Ln"/>
+        <filter val="4787 Wild Iris Dr 301"/>
+        <filter val="4846 Carnation Cir 105"/>
+        <filter val="4851 Luster Leaf Cir"/>
+        <filter val="4878 Dahlia Ct 301"/>
+        <filter val="488 River Oaks Dr 61E"/>
+        <filter val="4895 Luster Leaf Cir 105"/>
+        <filter val="4895 Luster Leaf Cir 205"/>
+        <filter val="6253 Catalina Dr"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0394ec80-3f17-43d0-8a0a-f2c35f612e53">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0b5c3551-8383-4165-8e29-fcb6c1524c16" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002833C68ECB254E46A2B1B064E5019715" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c333f1589930184ff6bd9e9abf6ec8fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0394EC80-3F17-43D0-8A0A-F2C35F612E53" xmlns:ns3="0394ec80-3f17-43d0-8a0a-f2c35f612e53" xmlns:ns4="385cac4a-83fd-4e8e-a4db-d44e8beb0c8f" xmlns:ns5="0b5c3551-8383-4165-8e29-fcb6c1524c16" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a043b4a353138303344697476d530922" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="0394EC80-3F17-43D0-8A0A-F2C35F612E53"/>
@@ -6105,28 +6175,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0394ec80-3f17-43d0-8a0a-f2c35f612e53">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0b5c3551-8383-4165-8e29-fcb6c1524c16" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D3693F1-EBC9-46E3-8A6A-9FB3C656A6F1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AE091A-8816-4226-806E-9B1AABFC3658}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6134,5 +6184,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AE091A-8816-4226-806E-9B1AABFC3658}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D3693F1-EBC9-46E3-8A6A-9FB3C656A6F1}"/>
 </file>
</xml_diff>